<commit_message>
update 507 581 577
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroup570_577_581.xlsx
+++ b/src/test/resources/data/jdgroup570_577_581.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="10" activeTab="13"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="42" activeTab="44"/>
   </bookViews>
   <sheets>
     <sheet name="evs_CreateaccountBackend++" sheetId="100" r:id="rId1"/>
@@ -21,82 +21,83 @@
     <sheet name="evs_Magento_UserInfoVerify++" sheetId="98" r:id="rId12"/>
     <sheet name="validatePaymentOption++" sheetId="95" r:id="rId13"/>
     <sheet name="EVS" sheetId="82" r:id="rId14"/>
-    <sheet name="evs_WishlistToCart++" sheetId="106" r:id="rId15"/>
-    <sheet name="evs_RemoveFromcart++" sheetId="105" r:id="rId16"/>
-    <sheet name="evs_ClearWishList++" sheetId="104" r:id="rId17"/>
-    <sheet name="evs_NavigetoWishlist++" sheetId="103" r:id="rId18"/>
-    <sheet name="evs_adminUserUpdate++" sheetId="102" r:id="rId19"/>
-    <sheet name="evs_UpdateUser++" sheetId="101" r:id="rId20"/>
-    <sheet name="evs_invalidCredslogin++" sheetId="97" r:id="rId21"/>
-    <sheet name="parallel_evs_Login++" sheetId="96" r:id="rId22"/>
-    <sheet name="evs_RetriveOrderID++" sheetId="91" r:id="rId23"/>
-    <sheet name="evs_PayUPagePayment++" sheetId="90" r:id="rId24"/>
-    <sheet name="evs_CheckoutpaymentOption++" sheetId="89" r:id="rId25"/>
-    <sheet name="evs_GenerateOrderSAPnumber++" sheetId="88" r:id="rId26"/>
-    <sheet name="evs_DeliveryPopulation++" sheetId="87" r:id="rId27"/>
-    <sheet name="evs_AccountCreation++" sheetId="86" r:id="rId28"/>
-    <sheet name="evs_ProductSearch++" sheetId="85" r:id="rId29"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId30"/>
-    <sheet name="accountCreation++" sheetId="39" r:id="rId31"/>
-    <sheet name="parrallel_ic_Login++" sheetId="84" r:id="rId32"/>
-    <sheet name="evs_InvalidEmailNewsLetter++" sheetId="109" r:id="rId33"/>
-    <sheet name="evs_Login++" sheetId="81" r:id="rId34"/>
-    <sheet name="SapRSIGetDataFromSAPDB++" sheetId="80" r:id="rId35"/>
-    <sheet name="icInvalidEmailNewsLetter++" sheetId="77" r:id="rId36"/>
-    <sheet name="evs_SubscribeNewsletter++" sheetId="110" r:id="rId37"/>
-    <sheet name="ic_SubscribeNewsletter++" sheetId="78" r:id="rId38"/>
-    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId39"/>
-    <sheet name="IC_ClearWishList++" sheetId="66" r:id="rId40"/>
-    <sheet name="ic_NavigetoWishlist++" sheetId="65" r:id="rId41"/>
-    <sheet name="Magento_UserInfoVerification++" sheetId="64" r:id="rId42"/>
-    <sheet name="IC_ProductsSortBy++" sheetId="63" r:id="rId43"/>
-    <sheet name="evs_SubscribeNews_DupEmailID++" sheetId="111" r:id="rId44"/>
-    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="62" r:id="rId45"/>
-    <sheet name="EnterSpouseInfor++" sheetId="61" r:id="rId46"/>
-    <sheet name="EnterContact++" sheetId="58" r:id="rId47"/>
-    <sheet name="CreditEnterAddressDetails++" sheetId="59" r:id="rId48"/>
-    <sheet name="CreditEnterEmploymentDetails++" sheetId="60" r:id="rId49"/>
-    <sheet name="EnterBasicDetails++" sheetId="57" r:id="rId50"/>
-    <sheet name="CreditStatusVerification++" sheetId="56" r:id="rId51"/>
-    <sheet name="CreditApp_NavigateFilter++" sheetId="55" r:id="rId52"/>
-    <sheet name="giftCardReport++" sheetId="54" r:id="rId53"/>
-    <sheet name="adminUserUpdate++" sheetId="52" r:id="rId54"/>
-    <sheet name="ICUpdateUser++" sheetId="51" r:id="rId55"/>
-    <sheet name="SapCustomer++" sheetId="50" r:id="rId56"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId57"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId58"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId59"/>
-    <sheet name="RetrieveCustomerDetailsOld++" sheetId="70" r:id="rId60"/>
-    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId61"/>
-    <sheet name="SAP_OrderRelated++" sheetId="46" r:id="rId62"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId63"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId64"/>
-    <sheet name="ic_RetriveOrderID++" sheetId="53" r:id="rId65"/>
-    <sheet name="IC_WishlistToCart++" sheetId="71" r:id="rId66"/>
-    <sheet name="Products_Category" sheetId="69" r:id="rId67"/>
-    <sheet name="icRedeemGiftCard++" sheetId="48" r:id="rId68"/>
-    <sheet name="VeriyGiftcardUsableity++" sheetId="49" r:id="rId69"/>
-    <sheet name="ic_login++" sheetId="44" r:id="rId70"/>
-    <sheet name="ClearCart++" sheetId="73" r:id="rId71"/>
-    <sheet name="ic_invalidCredslogin++" sheetId="74" r:id="rId72"/>
-    <sheet name="SendWishlistToEmail++" sheetId="75" r:id="rId73"/>
-    <sheet name="icEmailWishlistverification++" sheetId="76" r:id="rId74"/>
-    <sheet name="DB_connection_master++" sheetId="47" r:id="rId75"/>
-    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId76"/>
-    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId77"/>
-    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId78"/>
-    <sheet name="icSearchNoResultsReturned++" sheetId="79" r:id="rId79"/>
-    <sheet name="Russels" sheetId="26" r:id="rId80"/>
-    <sheet name="Login++" sheetId="25" r:id="rId81"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId82"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId83"/>
-    <sheet name="Preferred Store" sheetId="68" r:id="rId84"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId85"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId86"/>
+    <sheet name="evs_SubscribeNews_DupEmailI (2" sheetId="112" r:id="rId15"/>
+    <sheet name="evs_WishlistToCart++" sheetId="106" r:id="rId16"/>
+    <sheet name="evs_RemoveFromcart++" sheetId="105" r:id="rId17"/>
+    <sheet name="evs_ClearWishList++" sheetId="104" r:id="rId18"/>
+    <sheet name="evs_NavigetoWishlist++" sheetId="103" r:id="rId19"/>
+    <sheet name="evs_adminUserUpdate++" sheetId="102" r:id="rId20"/>
+    <sheet name="evs_UpdateUser++" sheetId="101" r:id="rId21"/>
+    <sheet name="evs_invalidCredslogin++" sheetId="97" r:id="rId22"/>
+    <sheet name="parallel_evs_Login++" sheetId="96" r:id="rId23"/>
+    <sheet name="evs_RetriveOrderID++" sheetId="91" r:id="rId24"/>
+    <sheet name="evs_PayUPagePayment++" sheetId="90" r:id="rId25"/>
+    <sheet name="evs_CheckoutpaymentOption++" sheetId="89" r:id="rId26"/>
+    <sheet name="evs_GenerateOrderSAPnumber++" sheetId="88" r:id="rId27"/>
+    <sheet name="evs_DeliveryPopulation++" sheetId="87" r:id="rId28"/>
+    <sheet name="evs_AccountCreation++" sheetId="86" r:id="rId29"/>
+    <sheet name="evs_ProductSearch++" sheetId="85" r:id="rId30"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId31"/>
+    <sheet name="accountCreation++" sheetId="39" r:id="rId32"/>
+    <sheet name="parrallel_ic_Login++" sheetId="84" r:id="rId33"/>
+    <sheet name="evs_InvalidEmailNewsLetter++" sheetId="109" r:id="rId34"/>
+    <sheet name="evs_Login++" sheetId="81" r:id="rId35"/>
+    <sheet name="SapRSIGetDataFromSAPDB++" sheetId="80" r:id="rId36"/>
+    <sheet name="icInvalidEmailNewsLetter++" sheetId="77" r:id="rId37"/>
+    <sheet name="evs_SubscribeNewsletter++" sheetId="110" r:id="rId38"/>
+    <sheet name="ic_SubscribeNewsletter++" sheetId="78" r:id="rId39"/>
+    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId40"/>
+    <sheet name="IC_ClearWishList++" sheetId="66" r:id="rId41"/>
+    <sheet name="ic_NavigetoWishlist++" sheetId="65" r:id="rId42"/>
+    <sheet name="Magento_UserInfoVerification++" sheetId="64" r:id="rId43"/>
+    <sheet name="IC_ProductsSortBy++" sheetId="63" r:id="rId44"/>
+    <sheet name="evs_SubscribeNews_DupEmailID++" sheetId="111" r:id="rId45"/>
+    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="62" r:id="rId46"/>
+    <sheet name="EnterSpouseInfor++" sheetId="61" r:id="rId47"/>
+    <sheet name="EnterContact++" sheetId="58" r:id="rId48"/>
+    <sheet name="CreditEnterAddressDetails++" sheetId="59" r:id="rId49"/>
+    <sheet name="CreditEnterEmploymentDetails++" sheetId="60" r:id="rId50"/>
+    <sheet name="EnterBasicDetails++" sheetId="57" r:id="rId51"/>
+    <sheet name="CreditStatusVerification++" sheetId="56" r:id="rId52"/>
+    <sheet name="CreditApp_NavigateFilter++" sheetId="55" r:id="rId53"/>
+    <sheet name="giftCardReport++" sheetId="54" r:id="rId54"/>
+    <sheet name="adminUserUpdate++" sheetId="52" r:id="rId55"/>
+    <sheet name="ICUpdateUser++" sheetId="51" r:id="rId56"/>
+    <sheet name="SapCustomer++" sheetId="50" r:id="rId57"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId58"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId59"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId60"/>
+    <sheet name="RetrieveCustomerDetailsOld++" sheetId="70" r:id="rId61"/>
+    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId62"/>
+    <sheet name="SAP_OrderRelated++" sheetId="46" r:id="rId63"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId64"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId65"/>
+    <sheet name="ic_RetriveOrderID++" sheetId="53" r:id="rId66"/>
+    <sheet name="IC_WishlistToCart++" sheetId="71" r:id="rId67"/>
+    <sheet name="Products_Category" sheetId="69" r:id="rId68"/>
+    <sheet name="icRedeemGiftCard++" sheetId="48" r:id="rId69"/>
+    <sheet name="VeriyGiftcardUsableity++" sheetId="49" r:id="rId70"/>
+    <sheet name="ic_login++" sheetId="44" r:id="rId71"/>
+    <sheet name="ClearCart++" sheetId="73" r:id="rId72"/>
+    <sheet name="ic_invalidCredslogin++" sheetId="74" r:id="rId73"/>
+    <sheet name="SendWishlistToEmail++" sheetId="75" r:id="rId74"/>
+    <sheet name="icEmailWishlistverification++" sheetId="76" r:id="rId75"/>
+    <sheet name="DB_connection_master++" sheetId="47" r:id="rId76"/>
+    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId77"/>
+    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId78"/>
+    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId79"/>
+    <sheet name="icSearchNoResultsReturned++" sheetId="79" r:id="rId80"/>
+    <sheet name="Russels" sheetId="26" r:id="rId81"/>
+    <sheet name="Login++" sheetId="25" r:id="rId82"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId83"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId84"/>
+    <sheet name="Preferred Store" sheetId="68" r:id="rId85"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId86"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId87"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId87"/>
     <externalReference r:id="rId88"/>
+    <externalReference r:id="rId89"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">IC!$A$1:$AH$94</definedName>
@@ -240,7 +241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4768" uniqueCount="956">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4777" uniqueCount="956">
   <si>
     <t>testSuitID</t>
   </si>
@@ -4000,7 +4001,17 @@
     <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="254">
+  <dxfs count="255">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -10706,121 +10717,121 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B53:B54">
-    <cfRule type="duplicateValues" dxfId="220" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="221" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="duplicateValues" dxfId="219" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="220" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="218" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="219" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:B52">
-    <cfRule type="duplicateValues" dxfId="217" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="218" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="duplicateValues" dxfId="216" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="217" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:A54 A2:A31 A33:A49">
-    <cfRule type="duplicateValues" dxfId="215" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="216" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="duplicateValues" dxfId="214" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="215" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="duplicateValues" dxfId="213" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="214" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="duplicateValues" dxfId="212" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="213" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74">
-    <cfRule type="duplicateValues" dxfId="211" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="212" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="duplicateValues" dxfId="210" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="211" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77">
-    <cfRule type="duplicateValues" dxfId="209" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="210" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78">
-    <cfRule type="duplicateValues" dxfId="208" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="209" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79">
-    <cfRule type="duplicateValues" dxfId="207" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="208" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58">
-    <cfRule type="duplicateValues" dxfId="206" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="207" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59">
-    <cfRule type="duplicateValues" dxfId="205" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="206" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60">
-    <cfRule type="duplicateValues" dxfId="204" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="205" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="duplicateValues" dxfId="203" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="204" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="duplicateValues" dxfId="202" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="203" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75">
-    <cfRule type="duplicateValues" dxfId="201" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="202" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D76">
-    <cfRule type="duplicateValues" dxfId="200" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="201" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D77">
-    <cfRule type="duplicateValues" dxfId="199" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="200" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="duplicateValues" dxfId="198" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="199" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D79">
-    <cfRule type="duplicateValues" dxfId="197" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="198" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95:B1048576 B81:B84 B33:B49 B1:B31 B55:B75">
-    <cfRule type="duplicateValues" dxfId="196" priority="90"/>
+    <cfRule type="duplicateValues" dxfId="197" priority="90"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72">
-    <cfRule type="duplicateValues" dxfId="195" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="196" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="duplicateValues" dxfId="194" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="195" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85">
-    <cfRule type="duplicateValues" dxfId="193" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="194" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86">
-    <cfRule type="duplicateValues" dxfId="192" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="193" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87">
-    <cfRule type="duplicateValues" dxfId="191" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="192" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87">
-    <cfRule type="duplicateValues" dxfId="190" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="191" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88:B92">
-    <cfRule type="duplicateValues" dxfId="189" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="190" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88:J91">
-    <cfRule type="duplicateValues" dxfId="188" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="189" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="duplicateValues" dxfId="187" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="188" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:D91">
-    <cfRule type="duplicateValues" dxfId="186" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="187" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="duplicateValues" dxfId="185" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="186" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92">
-    <cfRule type="duplicateValues" dxfId="184" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="185" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H92:H93">
-    <cfRule type="duplicateValues" dxfId="183" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="184" priority="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="duplicateValues" dxfId="182" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="183" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="I3" location="'Login_magento++'!A1" display="Login_magento"/>
@@ -11145,10 +11156,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="181" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="182" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="180" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="181" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -11434,10 +11445,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="179" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="180" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B18">
-    <cfRule type="duplicateValues" dxfId="178" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="179" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18">
@@ -11508,11 +11519,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C45" sqref="C45:C47"/>
+      <selection pane="bottomRight" activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -13077,70 +13088,70 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="177" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="178" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="176" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="177" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="175" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="176" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D7">
-    <cfRule type="duplicateValues" dxfId="174" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="175" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="173" priority="126"/>
+    <cfRule type="duplicateValues" dxfId="174" priority="126"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="172" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="173" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="171" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="172" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="170" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="171" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D23">
-    <cfRule type="duplicateValues" dxfId="169" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="170" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:D32">
-    <cfRule type="duplicateValues" dxfId="168" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="169" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B32">
-    <cfRule type="duplicateValues" dxfId="167" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="168" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:D37">
-    <cfRule type="duplicateValues" dxfId="166" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="167" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:B37">
-    <cfRule type="duplicateValues" dxfId="165" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="166" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="duplicateValues" dxfId="164" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="165" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="163" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41:B42">
-    <cfRule type="duplicateValues" dxfId="162" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="163" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="duplicateValues" dxfId="161" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="162" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="duplicateValues" dxfId="160" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="161" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="duplicateValues" dxfId="159" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="160" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:B47">
-    <cfRule type="duplicateValues" dxfId="158" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="159" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="duplicateValues" dxfId="157" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="158" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="duplicateValues" dxfId="156" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="157" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
@@ -13235,6 +13246,67 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="107" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" style="107" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="107" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="107" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="107" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="107"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="107" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="107" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1" s="107" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="227">
+        <v>44</v>
+      </c>
+      <c r="B2" s="121" t="s">
+        <v>528</v>
+      </c>
+      <c r="C2" s="107" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="107" t="s">
+        <v>380</v>
+      </c>
+      <c r="E2" s="107" t="s">
+        <v>381</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13309,13 +13381,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="155" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="156" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -13422,22 +13494,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="154" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="155" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="153" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="154" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B5">
-    <cfRule type="duplicateValues" dxfId="152" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="153" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="151" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="152" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="150" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="151" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="149" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -13446,7 +13518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -13589,25 +13661,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="148" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="149" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="147" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4 B6">
-    <cfRule type="duplicateValues" dxfId="146" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="147" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="145" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="146" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="144" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="145" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="143" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="142" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="143" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9">
@@ -13621,7 +13693,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -13802,19 +13874,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="141" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="142" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="140" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="141" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B5">
-    <cfRule type="duplicateValues" dxfId="139" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="138" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="139" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="137" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2:E3" r:id="rId1" display="watlevi41@gmail.com"/>
@@ -13827,7 +13899,345 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="176" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="188">
+        <v>16</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>890</v>
+      </c>
+      <c r="C2" s="110">
+        <v>1</v>
+      </c>
+      <c r="D2" s="190" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="199">
+        <v>17</v>
+      </c>
+      <c r="B3" s="203" t="s">
+        <v>876</v>
+      </c>
+      <c r="C3" s="110">
+        <v>1</v>
+      </c>
+      <c r="D3" s="190" t="s">
+        <v>208</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="188">
+        <v>18</v>
+      </c>
+      <c r="B4" s="203" t="s">
+        <v>877</v>
+      </c>
+      <c r="C4" s="110">
+        <v>1</v>
+      </c>
+      <c r="D4" s="190" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="199">
+        <v>19</v>
+      </c>
+      <c r="B5" s="203" t="s">
+        <v>878</v>
+      </c>
+      <c r="C5" s="110">
+        <v>1</v>
+      </c>
+      <c r="D5" s="190" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="21">
+        <v>24</v>
+      </c>
+      <c r="B6" s="201" t="s">
+        <v>905</v>
+      </c>
+      <c r="C6" s="110">
+        <v>1</v>
+      </c>
+      <c r="D6" s="190" t="s">
+        <v>245</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="21">
+        <v>25</v>
+      </c>
+      <c r="B7" s="202" t="s">
+        <v>907</v>
+      </c>
+      <c r="C7" s="110">
+        <v>1</v>
+      </c>
+      <c r="D7" s="190" t="s">
+        <v>245</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="21">
+        <v>26</v>
+      </c>
+      <c r="B8" s="202" t="s">
+        <v>908</v>
+      </c>
+      <c r="C8" s="110">
+        <v>1</v>
+      </c>
+      <c r="D8" s="190" t="s">
+        <v>245</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="198">
+        <v>27</v>
+      </c>
+      <c r="B9" s="209" t="s">
+        <v>924</v>
+      </c>
+      <c r="C9" s="110">
+        <v>1</v>
+      </c>
+      <c r="D9" s="190" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="198">
+        <v>28</v>
+      </c>
+      <c r="B10" s="210" t="s">
+        <v>926</v>
+      </c>
+      <c r="C10" s="110">
+        <v>1</v>
+      </c>
+      <c r="D10" s="190" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="198">
+        <v>29</v>
+      </c>
+      <c r="B11" s="210" t="s">
+        <v>927</v>
+      </c>
+      <c r="C11" s="110">
+        <v>1</v>
+      </c>
+      <c r="D11" s="190" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="198">
+        <v>30</v>
+      </c>
+      <c r="B12" s="210" t="s">
+        <v>928</v>
+      </c>
+      <c r="C12" s="110">
+        <v>1</v>
+      </c>
+      <c r="D12" s="190" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="198">
+        <v>31</v>
+      </c>
+      <c r="B13" s="210" t="s">
+        <v>929</v>
+      </c>
+      <c r="C13" s="110">
+        <v>1</v>
+      </c>
+      <c r="D13" s="190" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="198">
+        <v>32</v>
+      </c>
+      <c r="B14" s="118" t="s">
+        <v>501</v>
+      </c>
+      <c r="C14" s="110">
+        <v>1</v>
+      </c>
+      <c r="D14" s="190" t="s">
+        <v>209</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="198">
+        <v>33</v>
+      </c>
+      <c r="B15" s="118" t="s">
+        <v>516</v>
+      </c>
+      <c r="C15" s="110">
+        <v>1</v>
+      </c>
+      <c r="D15" s="190" t="s">
+        <v>209</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="198">
+        <v>34</v>
+      </c>
+      <c r="B16" s="118" t="s">
+        <v>517</v>
+      </c>
+      <c r="C16" s="110">
+        <v>1</v>
+      </c>
+      <c r="D16" s="190" t="s">
+        <v>209</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="198">
+        <v>35</v>
+      </c>
+      <c r="B17" s="118" t="s">
+        <v>518</v>
+      </c>
+      <c r="C17" s="110">
+        <v>1</v>
+      </c>
+      <c r="D17" s="190" t="s">
+        <v>209</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="198">
+        <v>36</v>
+      </c>
+      <c r="B18" s="118" t="s">
+        <v>519</v>
+      </c>
+      <c r="C18" s="110">
+        <v>1</v>
+      </c>
+      <c r="D18" s="190" t="s">
+        <v>209</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B14:B18">
+    <cfRule type="duplicateValues" dxfId="254" priority="1"/>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18">
+      <formula1>"Guest Customer Creation, Customer Creation, Customer Update,Customer Creation Magento Admin, Customer Update Magento Admin"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB8"/>
   <sheetViews>
@@ -14163,7 +14573,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="136" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="137" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R8">
@@ -14182,345 +14592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="30"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="176" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="188">
-        <v>16</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>890</v>
-      </c>
-      <c r="C2" s="110">
-        <v>1</v>
-      </c>
-      <c r="D2" s="190" t="s">
-        <v>208</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="199">
-        <v>17</v>
-      </c>
-      <c r="B3" s="203" t="s">
-        <v>876</v>
-      </c>
-      <c r="C3" s="110">
-        <v>1</v>
-      </c>
-      <c r="D3" s="190" t="s">
-        <v>208</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="188">
-        <v>18</v>
-      </c>
-      <c r="B4" s="203" t="s">
-        <v>877</v>
-      </c>
-      <c r="C4" s="110">
-        <v>1</v>
-      </c>
-      <c r="D4" s="190" t="s">
-        <v>208</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="199">
-        <v>19</v>
-      </c>
-      <c r="B5" s="203" t="s">
-        <v>878</v>
-      </c>
-      <c r="C5" s="110">
-        <v>1</v>
-      </c>
-      <c r="D5" s="190" t="s">
-        <v>208</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="21">
-        <v>24</v>
-      </c>
-      <c r="B6" s="201" t="s">
-        <v>905</v>
-      </c>
-      <c r="C6" s="110">
-        <v>1</v>
-      </c>
-      <c r="D6" s="190" t="s">
-        <v>245</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="21">
-        <v>25</v>
-      </c>
-      <c r="B7" s="202" t="s">
-        <v>907</v>
-      </c>
-      <c r="C7" s="110">
-        <v>1</v>
-      </c>
-      <c r="D7" s="190" t="s">
-        <v>245</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="21">
-        <v>26</v>
-      </c>
-      <c r="B8" s="202" t="s">
-        <v>908</v>
-      </c>
-      <c r="C8" s="110">
-        <v>1</v>
-      </c>
-      <c r="D8" s="190" t="s">
-        <v>245</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="198">
-        <v>27</v>
-      </c>
-      <c r="B9" s="209" t="s">
-        <v>924</v>
-      </c>
-      <c r="C9" s="110">
-        <v>1</v>
-      </c>
-      <c r="D9" s="190" t="s">
-        <v>207</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="198">
-        <v>28</v>
-      </c>
-      <c r="B10" s="210" t="s">
-        <v>926</v>
-      </c>
-      <c r="C10" s="110">
-        <v>1</v>
-      </c>
-      <c r="D10" s="190" t="s">
-        <v>207</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="198">
-        <v>29</v>
-      </c>
-      <c r="B11" s="210" t="s">
-        <v>927</v>
-      </c>
-      <c r="C11" s="110">
-        <v>1</v>
-      </c>
-      <c r="D11" s="190" t="s">
-        <v>207</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="198">
-        <v>30</v>
-      </c>
-      <c r="B12" s="210" t="s">
-        <v>928</v>
-      </c>
-      <c r="C12" s="110">
-        <v>1</v>
-      </c>
-      <c r="D12" s="190" t="s">
-        <v>207</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="198">
-        <v>31</v>
-      </c>
-      <c r="B13" s="210" t="s">
-        <v>929</v>
-      </c>
-      <c r="C13" s="110">
-        <v>1</v>
-      </c>
-      <c r="D13" s="190" t="s">
-        <v>207</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="198">
-        <v>32</v>
-      </c>
-      <c r="B14" s="118" t="s">
-        <v>501</v>
-      </c>
-      <c r="C14" s="110">
-        <v>1</v>
-      </c>
-      <c r="D14" s="190" t="s">
-        <v>209</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="198">
-        <v>33</v>
-      </c>
-      <c r="B15" s="118" t="s">
-        <v>516</v>
-      </c>
-      <c r="C15" s="110">
-        <v>1</v>
-      </c>
-      <c r="D15" s="190" t="s">
-        <v>209</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="198">
-        <v>34</v>
-      </c>
-      <c r="B16" s="118" t="s">
-        <v>517</v>
-      </c>
-      <c r="C16" s="110">
-        <v>1</v>
-      </c>
-      <c r="D16" s="190" t="s">
-        <v>209</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="198">
-        <v>35</v>
-      </c>
-      <c r="B17" s="118" t="s">
-        <v>518</v>
-      </c>
-      <c r="C17" s="110">
-        <v>1</v>
-      </c>
-      <c r="D17" s="190" t="s">
-        <v>209</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="198">
-        <v>36</v>
-      </c>
-      <c r="B18" s="118" t="s">
-        <v>519</v>
-      </c>
-      <c r="C18" s="110">
-        <v>1</v>
-      </c>
-      <c r="D18" s="190" t="s">
-        <v>209</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B14:B18">
-    <cfRule type="duplicateValues" dxfId="253" priority="1"/>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18">
-      <formula1>"Guest Customer Creation, Customer Creation, Customer Update,Customer Creation Magento Admin, Customer Update Magento Admin"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -14812,7 +14884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -14903,7 +14975,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="135" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
@@ -14916,7 +14988,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -15012,7 +15084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -15061,7 +15133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -15152,7 +15224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -15208,7 +15280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -15265,7 +15337,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="134" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="135" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -15274,7 +15346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -15415,7 +15487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T20"/>
   <sheetViews>
@@ -16177,7 +16249,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B16:B20">
-    <cfRule type="duplicateValues" dxfId="133" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="134" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q21:R22 P7 P2:T3 P10:P1048576 T7:T10 Q11:R17 S11:S15">
@@ -16208,7 +16280,57 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="99"/>
+    <col min="2" max="2" width="38.140625" style="99" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="99"/>
+    <col min="4" max="4" width="11.28515625" style="99" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="99"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30">
+      <c r="A1" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="99">
+        <v>1</v>
+      </c>
+      <c r="B2" s="99" t="s">
+        <v>820</v>
+      </c>
+      <c r="C2" s="99">
+        <v>1</v>
+      </c>
+      <c r="D2" s="99" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
@@ -16764,34 +16886,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="132" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="133" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="131" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="130" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="131" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="129" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="128" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="129" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="127" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="128" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="126" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="127" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="125" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="126" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="124" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="125" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="123" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="5"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G15">
@@ -16831,57 +16953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="99"/>
-    <col min="2" max="2" width="38.140625" style="99" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="99"/>
-    <col min="4" max="4" width="11.28515625" style="99" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="99"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="30">
-      <c r="A1" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="99">
-        <v>1</v>
-      </c>
-      <c r="B2" s="99" t="s">
-        <v>820</v>
-      </c>
-      <c r="C2" s="99">
-        <v>1</v>
-      </c>
-      <c r="D2" s="99" t="s">
-        <v>182</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
@@ -18170,34 +18242,34 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B15">
-    <cfRule type="duplicateValues" dxfId="122" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="121" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="duplicateValues" dxfId="120" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="119" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B33">
-    <cfRule type="duplicateValues" dxfId="118" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="117" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="116" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="duplicateValues" dxfId="115" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="duplicateValues" dxfId="114" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="113" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H16">
@@ -18237,7 +18309,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
@@ -19477,22 +19549,22 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A27">
-    <cfRule type="duplicateValues" dxfId="112" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="111" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B31">
-    <cfRule type="duplicateValues" dxfId="110" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A31">
-    <cfRule type="duplicateValues" dxfId="109" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B26">
-    <cfRule type="duplicateValues" dxfId="108" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A26">
-    <cfRule type="duplicateValues" dxfId="107" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="66"/>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11 M32">
@@ -19516,7 +19588,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -19613,7 +19685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -19628,7 +19700,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="57" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="84" t="s">
@@ -19657,16 +19729,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="106" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -19951,31 +20024,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B4">
-    <cfRule type="duplicateValues" dxfId="105" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="104" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="103" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:B13">
-    <cfRule type="duplicateValues" dxfId="102" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="101" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="100" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="101" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B17">
-    <cfRule type="duplicateValues" dxfId="99" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="98" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="97" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -19984,7 +20057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -20190,16 +20263,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="96" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="95" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -20247,13 +20320,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -20266,7 +20337,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="57" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="84" t="s">
@@ -20301,16 +20372,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="94" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="95" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="automation13@gmail.com"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -20362,111 +20434,6 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="79" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" style="79" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="79" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="79"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="79" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="79" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="79" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="78">
-        <v>52</v>
-      </c>
-      <c r="B2" s="78" t="s">
-        <v>527</v>
-      </c>
-      <c r="C2" s="79" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="78">
-        <v>53</v>
-      </c>
-      <c r="B3" s="78" t="s">
-        <v>526</v>
-      </c>
-      <c r="C3" s="79" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="56">
-        <v>54</v>
-      </c>
-      <c r="B4" s="63" t="s">
-        <v>603</v>
-      </c>
-      <c r="C4" s="79" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="77">
-        <v>55</v>
-      </c>
-      <c r="B5" s="63" t="s">
-        <v>602</v>
-      </c>
-      <c r="C5" s="79" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="56">
-        <v>56</v>
-      </c>
-      <c r="B6" s="63" t="s">
-        <v>604</v>
-      </c>
-      <c r="C6" s="79" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="77">
-        <v>70</v>
-      </c>
-      <c r="B7" s="63" t="s">
-        <v>616</v>
-      </c>
-      <c r="C7" s="79" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="93" priority="67"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="92" priority="69"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -20529,6 +20496,111 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="79" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="79" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="79" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="79"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="79" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="79" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="78">
+        <v>52</v>
+      </c>
+      <c r="B2" s="78" t="s">
+        <v>527</v>
+      </c>
+      <c r="C2" s="79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="78">
+        <v>53</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>526</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="56">
+        <v>54</v>
+      </c>
+      <c r="B4" s="63" t="s">
+        <v>603</v>
+      </c>
+      <c r="C4" s="79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="77">
+        <v>55</v>
+      </c>
+      <c r="B5" s="63" t="s">
+        <v>602</v>
+      </c>
+      <c r="C5" s="79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="56">
+        <v>56</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>604</v>
+      </c>
+      <c r="C6" s="79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="77">
+        <v>70</v>
+      </c>
+      <c r="B7" s="63" t="s">
+        <v>616</v>
+      </c>
+      <c r="C7" s="79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="94" priority="67"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="93" priority="69"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20672,16 +20744,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2 B4">
-    <cfRule type="duplicateValues" dxfId="91" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2 A4">
-    <cfRule type="duplicateValues" dxfId="90" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="91" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="89" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="88" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="89" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
@@ -20692,7 +20764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -20897,10 +20969,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="87" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="86" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
@@ -20917,7 +20989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -21292,22 +21364,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A21">
-    <cfRule type="duplicateValues" dxfId="85" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B21">
-    <cfRule type="duplicateValues" dxfId="84" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="83" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="82" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A26">
-    <cfRule type="duplicateValues" dxfId="81" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B26">
-    <cfRule type="duplicateValues" dxfId="80" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -21318,7 +21390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -21404,17 +21476,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="duplicateValues" dxfId="79" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -21462,13 +21534,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="78" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -21520,16 +21592,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="76" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -21680,10 +21752,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -21697,7 +21769,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -21808,10 +21880,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="73" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="72" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -21828,7 +21900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -21960,10 +22032,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="71" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="70" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
@@ -21986,7 +22058,140 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="166" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="101" t="s">
+        <v>774</v>
+      </c>
+      <c r="B1" s="101" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="101" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="101" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="101" t="s">
+        <v>795</v>
+      </c>
+      <c r="B2" s="101" t="s">
+        <v>722</v>
+      </c>
+      <c r="C2" s="101" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="101" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="101" t="s">
+        <v>796</v>
+      </c>
+      <c r="B3" s="101" t="s">
+        <v>798</v>
+      </c>
+      <c r="C3" s="101" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="101" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="101" t="s">
+        <v>797</v>
+      </c>
+      <c r="B4" s="101" t="s">
+        <v>722</v>
+      </c>
+      <c r="C4" s="126" t="s">
+        <v>597</v>
+      </c>
+      <c r="D4" s="101" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="101" t="s">
+        <v>782</v>
+      </c>
+      <c r="B5" s="180">
+        <v>225504</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>676</v>
+      </c>
+      <c r="D5" s="101" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="101" t="s">
+        <v>781</v>
+      </c>
+      <c r="B6" s="101" t="s">
+        <v>722</v>
+      </c>
+      <c r="C6" s="101" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="101" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="101" t="s">
+        <v>783</v>
+      </c>
+      <c r="B7" s="180">
+        <v>225504</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>676</v>
+      </c>
+      <c r="D7" s="101" t="s">
+        <v>778</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D6" r:id="rId2"/>
+    <hyperlink ref="D7" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="C6" r:id="rId6"/>
+    <hyperlink ref="D3" r:id="rId7"/>
+    <hyperlink ref="C3" r:id="rId8"/>
+    <hyperlink ref="D4" r:id="rId9"/>
+    <hyperlink ref="C4" r:id="rId10"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -22087,10 +22292,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="69" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -22102,140 +22307,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="32" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="166" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="30"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="101" t="s">
-        <v>774</v>
-      </c>
-      <c r="B1" s="101" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="101" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="101" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="101" t="s">
-        <v>795</v>
-      </c>
-      <c r="B2" s="101" t="s">
-        <v>722</v>
-      </c>
-      <c r="C2" s="101" t="s">
-        <v>166</v>
-      </c>
-      <c r="D2" s="101" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="101" t="s">
-        <v>796</v>
-      </c>
-      <c r="B3" s="101" t="s">
-        <v>798</v>
-      </c>
-      <c r="C3" s="101" t="s">
-        <v>166</v>
-      </c>
-      <c r="D3" s="101" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="101" t="s">
-        <v>797</v>
-      </c>
-      <c r="B4" s="101" t="s">
-        <v>722</v>
-      </c>
-      <c r="C4" s="126" t="s">
-        <v>597</v>
-      </c>
-      <c r="D4" s="101" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="101" t="s">
-        <v>782</v>
-      </c>
-      <c r="B5" s="180">
-        <v>225504</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>676</v>
-      </c>
-      <c r="D5" s="101" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="101" t="s">
-        <v>781</v>
-      </c>
-      <c r="B6" s="101" t="s">
-        <v>722</v>
-      </c>
-      <c r="C6" s="101" t="s">
-        <v>166</v>
-      </c>
-      <c r="D6" s="101" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="101" t="s">
-        <v>783</v>
-      </c>
-      <c r="B7" s="180">
-        <v>225504</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>676</v>
-      </c>
-      <c r="D7" s="101" t="s">
-        <v>778</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D6" r:id="rId2"/>
-    <hyperlink ref="D7" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
-    <hyperlink ref="C6" r:id="rId6"/>
-    <hyperlink ref="D3" r:id="rId7"/>
-    <hyperlink ref="C3" r:id="rId8"/>
-    <hyperlink ref="D4" r:id="rId9"/>
-    <hyperlink ref="C4" r:id="rId10"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -22476,10 +22548,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="67" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="66" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3">
@@ -22509,7 +22581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -22571,16 +22643,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="65" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="64" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -22626,16 +22698,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="63" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="62" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -22726,7 +22798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
@@ -23359,22 +23431,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="61" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="60" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="59" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="58" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="57" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="56" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="47"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10">
@@ -23394,7 +23466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
@@ -24035,22 +24107,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="55" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="54" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="53" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="52" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="51" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="50" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="29"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576">
@@ -24061,7 +24133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -24510,10 +24582,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="49" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="48" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -24524,7 +24596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
@@ -25022,13 +25094,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="duplicateValues" dxfId="47" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -25038,7 +25110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -25292,13 +25364,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="44" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="43" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="42" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -25312,7 +25384,406 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="176" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>784</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="30">
+        <v>1</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>820</v>
+      </c>
+      <c r="C2" s="180">
+        <v>1</v>
+      </c>
+      <c r="D2" s="180" t="s">
+        <v>783</v>
+      </c>
+      <c r="E2" s="180">
+        <v>225504</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="30">
+        <v>7</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>838</v>
+      </c>
+      <c r="C3" s="30">
+        <v>1</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>783</v>
+      </c>
+      <c r="E3" s="30">
+        <v>225504</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="188">
+        <v>16</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>872</v>
+      </c>
+      <c r="C4" s="30">
+        <v>1</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="199">
+        <v>17</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>876</v>
+      </c>
+      <c r="C5" s="30">
+        <v>1</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="188">
+        <v>18</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>877</v>
+      </c>
+      <c r="C6" s="30">
+        <v>1</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="199">
+        <v>19</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>878</v>
+      </c>
+      <c r="C7" s="30">
+        <v>1</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="21">
+        <v>24</v>
+      </c>
+      <c r="B8" s="201" t="s">
+        <v>905</v>
+      </c>
+      <c r="C8" s="30">
+        <v>1</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="21">
+        <v>25</v>
+      </c>
+      <c r="B9" s="202" t="s">
+        <v>907</v>
+      </c>
+      <c r="C9" s="30">
+        <v>1</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="21">
+        <v>26</v>
+      </c>
+      <c r="B10" s="202" t="s">
+        <v>908</v>
+      </c>
+      <c r="C10" s="30">
+        <v>1</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="99" customFormat="1">
+      <c r="A11" s="21">
+        <v>20</v>
+      </c>
+      <c r="B11" s="111" t="s">
+        <v>501</v>
+      </c>
+      <c r="C11" s="99">
+        <v>1</v>
+      </c>
+      <c r="D11" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="99" customFormat="1">
+      <c r="A12" s="21">
+        <v>21</v>
+      </c>
+      <c r="B12" s="111" t="s">
+        <v>516</v>
+      </c>
+      <c r="C12" s="99">
+        <v>1</v>
+      </c>
+      <c r="D12" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="99" customFormat="1">
+      <c r="A13" s="21">
+        <v>22</v>
+      </c>
+      <c r="B13" s="111" t="s">
+        <v>517</v>
+      </c>
+      <c r="C13" s="99">
+        <v>1</v>
+      </c>
+      <c r="D13" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="99" customFormat="1">
+      <c r="A14" s="21">
+        <v>23</v>
+      </c>
+      <c r="B14" s="111" t="s">
+        <v>518</v>
+      </c>
+      <c r="C14" s="99">
+        <v>1</v>
+      </c>
+      <c r="D14" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="99" customFormat="1">
+      <c r="A15" s="188">
+        <v>24</v>
+      </c>
+      <c r="B15" s="111" t="s">
+        <v>519</v>
+      </c>
+      <c r="C15" s="99">
+        <v>1</v>
+      </c>
+      <c r="D15" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="99" customFormat="1">
+      <c r="A16" s="198">
+        <v>27</v>
+      </c>
+      <c r="B16" s="207" t="s">
+        <v>924</v>
+      </c>
+      <c r="C16" s="99">
+        <v>1</v>
+      </c>
+      <c r="D16" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="99" customFormat="1">
+      <c r="A17" s="198">
+        <v>28</v>
+      </c>
+      <c r="B17" s="208" t="s">
+        <v>926</v>
+      </c>
+      <c r="C17" s="99">
+        <v>1</v>
+      </c>
+      <c r="D17" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="99" customFormat="1">
+      <c r="A18" s="198">
+        <v>29</v>
+      </c>
+      <c r="B18" s="208" t="s">
+        <v>927</v>
+      </c>
+      <c r="C18" s="99">
+        <v>1</v>
+      </c>
+      <c r="D18" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="99" customFormat="1">
+      <c r="A19" s="198">
+        <v>30</v>
+      </c>
+      <c r="B19" s="208" t="s">
+        <v>928</v>
+      </c>
+      <c r="C19" s="99">
+        <v>1</v>
+      </c>
+      <c r="D19" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="99" customFormat="1">
+      <c r="A20" s="198">
+        <v>31</v>
+      </c>
+      <c r="B20" s="208" t="s">
+        <v>929</v>
+      </c>
+      <c r="C20" s="99">
+        <v>1</v>
+      </c>
+      <c r="D20" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="99" customFormat="1">
+      <c r="A21" s="198">
+        <v>32</v>
+      </c>
+      <c r="B21" s="111" t="s">
+        <v>501</v>
+      </c>
+      <c r="C21" s="99">
+        <v>1</v>
+      </c>
+      <c r="D21" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="99" customFormat="1">
+      <c r="A22" s="198">
+        <v>33</v>
+      </c>
+      <c r="B22" s="111" t="s">
+        <v>516</v>
+      </c>
+      <c r="C22" s="99">
+        <v>1</v>
+      </c>
+      <c r="D22" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="99" customFormat="1">
+      <c r="A23" s="198">
+        <v>34</v>
+      </c>
+      <c r="B23" s="111" t="s">
+        <v>517</v>
+      </c>
+      <c r="C23" s="99">
+        <v>1</v>
+      </c>
+      <c r="D23" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="99" customFormat="1">
+      <c r="A24" s="198">
+        <v>35</v>
+      </c>
+      <c r="B24" s="111" t="s">
+        <v>518</v>
+      </c>
+      <c r="C24" s="99">
+        <v>1</v>
+      </c>
+      <c r="D24" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="99" customFormat="1">
+      <c r="A25" s="198">
+        <v>36</v>
+      </c>
+      <c r="B25" s="111" t="s">
+        <v>519</v>
+      </c>
+      <c r="C25" s="99">
+        <v>1</v>
+      </c>
+      <c r="D25" s="99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B11:B15">
+    <cfRule type="duplicateValues" dxfId="253" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:B25">
+    <cfRule type="duplicateValues" dxfId="252" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P35"/>
   <sheetViews>
@@ -26266,16 +26737,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="duplicateValues" dxfId="41" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="40" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B33">
-    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A33">
-    <cfRule type="duplicateValues" dxfId="38" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1"/>
@@ -26295,406 +26766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="30"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="176" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>784</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="30">
-        <v>1</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>820</v>
-      </c>
-      <c r="C2" s="180">
-        <v>1</v>
-      </c>
-      <c r="D2" s="180" t="s">
-        <v>783</v>
-      </c>
-      <c r="E2" s="180">
-        <v>225504</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="30">
-        <v>7</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>838</v>
-      </c>
-      <c r="C3" s="30">
-        <v>1</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>783</v>
-      </c>
-      <c r="E3" s="30">
-        <v>225504</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="188">
-        <v>16</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>872</v>
-      </c>
-      <c r="C4" s="30">
-        <v>1</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="199">
-        <v>17</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>876</v>
-      </c>
-      <c r="C5" s="30">
-        <v>1</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="188">
-        <v>18</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>877</v>
-      </c>
-      <c r="C6" s="30">
-        <v>1</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="199">
-        <v>19</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C7" s="30">
-        <v>1</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="21">
-        <v>24</v>
-      </c>
-      <c r="B8" s="201" t="s">
-        <v>905</v>
-      </c>
-      <c r="C8" s="30">
-        <v>1</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="21">
-        <v>25</v>
-      </c>
-      <c r="B9" s="202" t="s">
-        <v>907</v>
-      </c>
-      <c r="C9" s="30">
-        <v>1</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="21">
-        <v>26</v>
-      </c>
-      <c r="B10" s="202" t="s">
-        <v>908</v>
-      </c>
-      <c r="C10" s="30">
-        <v>1</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="99" customFormat="1">
-      <c r="A11" s="21">
-        <v>20</v>
-      </c>
-      <c r="B11" s="111" t="s">
-        <v>501</v>
-      </c>
-      <c r="C11" s="99">
-        <v>1</v>
-      </c>
-      <c r="D11" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="99" customFormat="1">
-      <c r="A12" s="21">
-        <v>21</v>
-      </c>
-      <c r="B12" s="111" t="s">
-        <v>516</v>
-      </c>
-      <c r="C12" s="99">
-        <v>1</v>
-      </c>
-      <c r="D12" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="99" customFormat="1">
-      <c r="A13" s="21">
-        <v>22</v>
-      </c>
-      <c r="B13" s="111" t="s">
-        <v>517</v>
-      </c>
-      <c r="C13" s="99">
-        <v>1</v>
-      </c>
-      <c r="D13" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="99" customFormat="1">
-      <c r="A14" s="21">
-        <v>23</v>
-      </c>
-      <c r="B14" s="111" t="s">
-        <v>518</v>
-      </c>
-      <c r="C14" s="99">
-        <v>1</v>
-      </c>
-      <c r="D14" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="99" customFormat="1">
-      <c r="A15" s="188">
-        <v>24</v>
-      </c>
-      <c r="B15" s="111" t="s">
-        <v>519</v>
-      </c>
-      <c r="C15" s="99">
-        <v>1</v>
-      </c>
-      <c r="D15" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="99" customFormat="1">
-      <c r="A16" s="198">
-        <v>27</v>
-      </c>
-      <c r="B16" s="207" t="s">
-        <v>924</v>
-      </c>
-      <c r="C16" s="99">
-        <v>1</v>
-      </c>
-      <c r="D16" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="99" customFormat="1">
-      <c r="A17" s="198">
-        <v>28</v>
-      </c>
-      <c r="B17" s="208" t="s">
-        <v>926</v>
-      </c>
-      <c r="C17" s="99">
-        <v>1</v>
-      </c>
-      <c r="D17" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="99" customFormat="1">
-      <c r="A18" s="198">
-        <v>29</v>
-      </c>
-      <c r="B18" s="208" t="s">
-        <v>927</v>
-      </c>
-      <c r="C18" s="99">
-        <v>1</v>
-      </c>
-      <c r="D18" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="99" customFormat="1">
-      <c r="A19" s="198">
-        <v>30</v>
-      </c>
-      <c r="B19" s="208" t="s">
-        <v>928</v>
-      </c>
-      <c r="C19" s="99">
-        <v>1</v>
-      </c>
-      <c r="D19" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="99" customFormat="1">
-      <c r="A20" s="198">
-        <v>31</v>
-      </c>
-      <c r="B20" s="208" t="s">
-        <v>929</v>
-      </c>
-      <c r="C20" s="99">
-        <v>1</v>
-      </c>
-      <c r="D20" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="99" customFormat="1">
-      <c r="A21" s="198">
-        <v>32</v>
-      </c>
-      <c r="B21" s="111" t="s">
-        <v>501</v>
-      </c>
-      <c r="C21" s="99">
-        <v>1</v>
-      </c>
-      <c r="D21" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="99" customFormat="1">
-      <c r="A22" s="198">
-        <v>33</v>
-      </c>
-      <c r="B22" s="111" t="s">
-        <v>516</v>
-      </c>
-      <c r="C22" s="99">
-        <v>1</v>
-      </c>
-      <c r="D22" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="99" customFormat="1">
-      <c r="A23" s="198">
-        <v>34</v>
-      </c>
-      <c r="B23" s="111" t="s">
-        <v>517</v>
-      </c>
-      <c r="C23" s="99">
-        <v>1</v>
-      </c>
-      <c r="D23" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="99" customFormat="1">
-      <c r="A24" s="198">
-        <v>35</v>
-      </c>
-      <c r="B24" s="111" t="s">
-        <v>518</v>
-      </c>
-      <c r="C24" s="99">
-        <v>1</v>
-      </c>
-      <c r="D24" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="99" customFormat="1">
-      <c r="A25" s="198">
-        <v>36</v>
-      </c>
-      <c r="B25" s="111" t="s">
-        <v>519</v>
-      </c>
-      <c r="C25" s="99">
-        <v>1</v>
-      </c>
-      <c r="D25" s="99" t="s">
-        <v>783</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B11:B15">
-    <cfRule type="duplicateValues" dxfId="252" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21:B25">
-    <cfRule type="duplicateValues" dxfId="251" priority="1"/>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -26849,22 +26921,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A6">
-    <cfRule type="duplicateValues" dxfId="36" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B12">
-    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A12">
-    <cfRule type="duplicateValues" dxfId="34" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -27039,7 +27111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -27277,10 +27349,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A13">
-    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -27289,7 +27361,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -27579,13 +27651,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="31" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="30" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="29" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -27594,7 +27666,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -27881,13 +27953,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="28" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="27" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="26" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -27896,7 +27968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -28130,22 +28202,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="25" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="24" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="23" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="22" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="21" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -28154,7 +28226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -28217,7 +28289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A18"/>
   <sheetViews>
@@ -28325,7 +28397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -28432,90 +28504,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>34</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1">
-      <c r="A3" s="1">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>100</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -29518,67 +29506,67 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B49:B52 B29:B44 B18:B23 B2:B16">
-    <cfRule type="duplicateValues" dxfId="250" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="251" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="249" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="250" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:B28">
-    <cfRule type="duplicateValues" dxfId="248" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="249" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B26">
-    <cfRule type="duplicateValues" dxfId="247" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="248" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="duplicateValues" dxfId="246" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="247" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="duplicateValues" dxfId="245" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="246" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="duplicateValues" dxfId="244" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="245" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="duplicateValues" dxfId="243" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="244" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="duplicateValues" dxfId="242" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="243" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="duplicateValues" dxfId="241" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="242" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55:B59">
-    <cfRule type="duplicateValues" dxfId="240" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="241" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="duplicateValues" dxfId="239" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="240" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A60">
-    <cfRule type="duplicateValues" dxfId="238" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="239" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
-    <cfRule type="duplicateValues" dxfId="237" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="238" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:A67">
-    <cfRule type="duplicateValues" dxfId="236" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="237" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="duplicateValues" dxfId="235" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="236" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63">
-    <cfRule type="duplicateValues" dxfId="234" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="235" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65:B66">
-    <cfRule type="duplicateValues" dxfId="233" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="234" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67">
-    <cfRule type="duplicateValues" dxfId="232" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="233" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68">
-    <cfRule type="duplicateValues" dxfId="231" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="232" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69:B70">
-    <cfRule type="duplicateValues" dxfId="230" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="231" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -29594,6 +29582,90 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>100</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
@@ -30180,25 +30252,25 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B16">
-    <cfRule type="duplicateValues" dxfId="19" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="duplicateValues" dxfId="18" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="duplicateValues" dxfId="17" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:B21">
-    <cfRule type="duplicateValues" dxfId="16" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="duplicateValues" dxfId="15" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -30245,7 +30317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -30439,25 +30511,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9:B12">
-    <cfRule type="duplicateValues" dxfId="12" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:A12">
-    <cfRule type="duplicateValues" dxfId="11" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="10" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B7">
-    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -30466,7 +30538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -30561,7 +30633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -30617,7 +30689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -30725,7 +30797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -30857,7 +30929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -30994,7 +31066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -31051,7 +31123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
@@ -31503,22 +31575,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B21">
-    <cfRule type="duplicateValues" dxfId="1" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A21">
-    <cfRule type="duplicateValues" dxfId="0" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="56"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
@@ -31536,47 +31608,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
   <legacyDrawing r:id="rId5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>44</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>710</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -32164,31 +32195,31 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B33:B35">
-    <cfRule type="duplicateValues" dxfId="229" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="230" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="duplicateValues" dxfId="228" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="229" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="227" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="228" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:A32">
-    <cfRule type="duplicateValues" dxfId="226" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="227" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:B32">
-    <cfRule type="duplicateValues" dxfId="225" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="226" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="duplicateValues" dxfId="224" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="225" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="duplicateValues" dxfId="223" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="224" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="222" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="223" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="duplicateValues" dxfId="221" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="222" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -32199,6 +32230,47 @@
 </file>
 
 <file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>710</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -32302,7 +32374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -32503,110 +32575,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -32716,6 +32684,110 @@
 
 <file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -33087,7 +33159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -33191,7 +33263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>

</xml_diff>